<commit_message>
Update Model creation for Sanity check
</commit_message>
<xml_diff>
--- a/test/testcase/Sales Order Data model.xlsx
+++ b/test/testcase/Sales Order Data model.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="450" windowWidth="16995" windowHeight="7395"/>
+    <workbookView xWindow="12820" yWindow="2720" windowWidth="25320" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrder" sheetId="1" r:id="rId1"/>
     <sheet name="SalesOrderItem" sheetId="2" r:id="rId2"/>
     <sheet name="Product" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -210,9 +215,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>ProductID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -222,7 +224,10 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>SalesOrderID</t>
+    <t>SalesOrder.SalesOrderSet.salesorderitem</t>
+  </si>
+  <si>
+    <t>SalesOrderItem.Relation.Product</t>
   </si>
 </sst>
 </file>
@@ -565,36 +570,36 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -603,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -623,7 +628,7 @@
         <v>42027</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -643,7 +648,7 @@
         <v>42028</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -663,7 +668,7 @@
         <v>42029</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -685,6 +690,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -693,34 +703,35 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -734,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -748,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -762,7 +773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -776,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -790,7 +801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -804,7 +815,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -818,7 +829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -832,7 +843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -846,7 +857,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -860,7 +871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -874,7 +885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -890,6 +901,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -901,21 +917,21 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -923,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -932,7 +948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -949,7 +965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -966,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -983,7 +999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1000,7 +1016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1017,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1034,7 +1050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1051,7 +1067,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1068,7 +1084,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1085,7 +1101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1102,7 +1118,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1121,5 +1137,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Sanity Excel file to be align with last dev
Change-Id: I44370361454cac55bf402ba59c52990ce496bdad
</commit_message>
<xml_diff>
--- a/test/testcase/Sales Order Data model.xlsx
+++ b/test/testcase/Sales Order Data model.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="2720" windowWidth="25320" windowHeight="13620"/>
+    <workbookView xWindow="12825" yWindow="2715" windowWidth="25320" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrder" sheetId="1" r:id="rId1"/>
@@ -224,10 +224,10 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>SalesOrder.SalesOrderSet.salesorderitem</t>
-  </si>
-  <si>
     <t>SalesOrderItem.Relation.Product</t>
+  </si>
+  <si>
+    <t>SalesOrder.SalesOrderSet.SalesOrderItem</t>
   </si>
 </sst>
 </file>
@@ -569,26 +569,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -628,7 +628,7 @@
         <v>42027</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -648,7 +648,7 @@
         <v>42028</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -668,7 +668,7 @@
         <v>42029</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -702,22 +702,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -725,13 +725,13 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -745,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -759,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -773,7 +773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -787,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -801,7 +801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -815,7 +815,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -829,7 +829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -843,7 +843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -857,7 +857,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -871,7 +871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -885,7 +885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -917,21 +917,21 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -948,7 +948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -965,7 +965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -982,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -999,7 +999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Update SanityCheck for DataModeler
Change-Id: I7f275ded340eb368d0143be7dcc6eddef85801d8
</commit_message>
<xml_diff>
--- a/test/testcase/Sales Order Data model.xlsx
+++ b/test/testcase/Sales Order Data model.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -206,15 +206,6 @@
     <t>D11</t>
   </si>
   <si>
-    <t>SalesOrder</t>
-  </si>
-  <si>
-    <t>SalesOrderItem</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -224,10 +215,10 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>SalesOrderItem.Relation.Product</t>
-  </si>
-  <si>
-    <t>SalesOrder.SalesOrderSet.SalesOrderItem</t>
+    <t>SalesOrder.SalesOrderItem.SalesOrderItem</t>
+  </si>
+  <si>
+    <t>SalesOrderItem.RelationName.Product</t>
   </si>
 </sst>
 </file>
@@ -567,39 +558,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -700,35 +686,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,11 +894,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -926,11 +907,6 @@
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
@@ -939,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>

</xml_diff>